<commit_message>
Added manuscript and update model code
</commit_message>
<xml_diff>
--- a/Experimental Results/dilution rate measurements.xlsx
+++ b/Experimental Results/dilution rate measurements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="132" windowWidth="14340" windowHeight="5832" activeTab="1"/>
+    <workbookView xWindow="390" yWindow="135" windowWidth="14340" windowHeight="5835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="10_22" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>Liters</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t xml:space="preserve">OD: </t>
+  </si>
+  <si>
+    <t>z-score</t>
+  </si>
+  <si>
+    <t>Flow rate (mmol/hr)</t>
+  </si>
+  <si>
+    <t>Flux (mmol/g(DCW)/hr</t>
   </si>
 </sst>
 </file>
@@ -472,19 +481,19 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -492,12 +501,12 @@
         <v>0.626</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -514,7 +523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f>26+20/60</f>
         <v>26.333333333333332</v>
@@ -541,7 +550,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>22+1/12</f>
         <v>22.083333333333332</v>
@@ -562,7 +571,7 @@
         <v>8.0313278746885014E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <f>25+10/60</f>
         <v>25.166666666666668</v>
@@ -583,7 +592,7 @@
         <v>8.2469074097213532E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
@@ -592,7 +601,7 @@
         <v>8.1391176422049266E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="4" t="s">
         <v>17</v>
       </c>
@@ -601,7 +610,7 @@
         <v>1.5243775110677241E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -609,7 +618,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -620,7 +629,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12.84</v>
       </c>
@@ -632,7 +641,7 @@
         <v>14540</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12.7</v>
       </c>
@@ -644,7 +653,7 @@
         <v>14297</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12.55</v>
       </c>
@@ -656,7 +665,7 @@
         <v>14693</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12.36</v>
       </c>
@@ -665,7 +674,7 @@
         <v>242.71844660194179</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>12.93</v>
       </c>
@@ -674,7 +683,7 @@
         <v>232.01856148491879</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -683,7 +692,7 @@
         <v>236.72923300841694</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>14</v>
       </c>
@@ -699,7 +708,7 @@
         <v>14510</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E19" s="4" t="s">
         <v>15</v>
       </c>
@@ -715,22 +724,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -738,12 +747,12 @@
         <v>0.67200000000000004</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -760,7 +769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <f>25+55/60</f>
         <v>25.916666666666668</v>
@@ -784,7 +793,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>23+23/60</f>
         <v>23.383333333333333</v>
@@ -805,7 +814,7 @@
         <v>9.9248241638537363E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>24</v>
       </c>
@@ -825,7 +834,7 @@
         <v>8.4119496855345893E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
@@ -834,7 +843,7 @@
         <v>9.1683869246941635E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="4" t="s">
         <v>17</v>
       </c>
@@ -843,7 +852,7 @@
         <v>1.0697638027035293E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -851,7 +860,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -861,8 +870,11 @@
       <c r="F11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12.25</v>
       </c>
@@ -873,8 +885,12 @@
       <c r="F12">
         <v>14371</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <f>(F12-$F$18)/$F$19</f>
+        <v>0.48690612102124614</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11.74</v>
       </c>
@@ -885,8 +901,12 @@
       <c r="F13">
         <v>14899</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <f t="shared" ref="G13:G16" si="4">(F13-$F$18)/$F$19</f>
+        <v>0.95096105224727134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12.08</v>
       </c>
@@ -897,8 +917,12 @@
       <c r="F14">
         <v>11940</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <f t="shared" si="4"/>
+        <v>-1.6496801248319115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12.4</v>
       </c>
@@ -909,8 +933,12 @@
       <c r="F15">
         <v>13665</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G15">
+        <f t="shared" si="4"/>
+        <v>-0.13359157111052242</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>11.83</v>
       </c>
@@ -921,8 +949,12 @@
       <c r="F16">
         <v>14210</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G16">
+        <f t="shared" si="4"/>
+        <v>0.34540452267391647</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -931,7 +963,7 @@
         <v>248.86140042339238</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>14</v>
       </c>
@@ -947,13 +979,31 @@
         <v>13817</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E19" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F19" s="5">
         <f>STDEV(F12:F16)</f>
         <v>1137.7963350266164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <f>B17*60/1000/22.4</f>
+        <v>0.66659303684837246</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <f>B20/B1</f>
+        <v>0.99195392388150661</v>
       </c>
     </row>
   </sheetData>
@@ -967,7 +1017,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated to 11_12 measurements
</commit_message>
<xml_diff>
--- a/Experimental Results/dilution rate measurements.xlsx
+++ b/Experimental Results/dilution rate measurements.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="132" windowWidth="14340" windowHeight="5832" activeTab="3"/>
+    <workbookView xWindow="384" yWindow="132" windowWidth="14340" windowHeight="5832" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="10_22" sheetId="1" r:id="rId1"/>
     <sheet name="10_27" sheetId="2" r:id="rId2"/>
     <sheet name="11_2" sheetId="3" r:id="rId3"/>
     <sheet name="11_5" sheetId="4" r:id="rId4"/>
+    <sheet name="11_12" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="19">
   <si>
     <t>Liters</t>
   </si>
@@ -1229,6 +1230,249 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1">
+        <v>0.67200000000000004</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <f>24+7+3/4</f>
+        <v>31.75</v>
+      </c>
+      <c r="B4" s="6">
+        <v>3.55</v>
+      </c>
+      <c r="C4" s="6">
+        <f>B4/2.65</f>
+        <v>1.3396226415094339</v>
+      </c>
+      <c r="D4" s="6">
+        <f>A4/C4</f>
+        <v>23.700704225352116</v>
+      </c>
+      <c r="E4" s="6">
+        <f>1/D4</f>
+        <v>4.2192839102659335E-2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f>24+40/60</f>
+        <v>24.666666666666668</v>
+      </c>
+      <c r="B5">
+        <v>3.125</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C6" si="0">B5/2.65</f>
+        <v>1.179245283018868</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D6" si="1">A5/C5</f>
+        <v>20.917333333333332</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E6" si="2">1/D5</f>
+        <v>4.7807241203467625E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <f>48+20+0.25</f>
+        <v>68.25</v>
+      </c>
+      <c r="B6">
+        <v>8.35</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>3.1509433962264151</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>21.660179640718564</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>4.616766880917824E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3">
+        <f>AVERAGE(E4:E6)</f>
+        <v>4.538924970510174E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="5">
+        <f>STDEV(E4:E6)</f>
+        <v>2.8870105582736597E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>12.48</v>
+      </c>
+      <c r="B12">
+        <f>50/A12*60</f>
+        <v>240.38461538461539</v>
+      </c>
+      <c r="F12">
+        <v>13870</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12.45</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ref="B13:B16" si="3">50/A13*60</f>
+        <v>240.96385542168676</v>
+      </c>
+      <c r="F13">
+        <v>14880</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12.59</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="3"/>
+        <v>238.28435266084193</v>
+      </c>
+      <c r="F14">
+        <v>14742</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>12.57</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="3"/>
+        <v>238.6634844868735</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>12.36</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="3"/>
+        <v>242.71844660194179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="3">
+        <f>AVERAGE(B12:B16)</f>
+        <v>240.20295091119186</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="5">
+        <f>STDEV(B12:B16)</f>
+        <v>1.8021287650322444</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="3">
+        <f>AVERAGE(F12:F16)</f>
+        <v>14497.333333333334</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="5">
+        <f>STDEV(F12:F16)</f>
+        <v>547.65074028374454</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
@@ -1247,7 +1491,7 @@
         <v>18</v>
       </c>
       <c r="B1">
-        <v>0.67200000000000004</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1358,56 +1602,56 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>12.48</v>
+        <v>12.8</v>
       </c>
       <c r="B12">
         <f>50/A12*60</f>
-        <v>240.38461538461539</v>
+        <v>234.375</v>
       </c>
       <c r="F12">
-        <v>13870</v>
+        <v>10464</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>12.45</v>
+        <v>12.81</v>
       </c>
       <c r="B13">
         <f t="shared" ref="B13:B16" si="3">50/A13*60</f>
-        <v>240.96385542168676</v>
+        <v>234.19203747072598</v>
       </c>
       <c r="F13">
-        <v>14880</v>
+        <v>10676</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>12.59</v>
+        <v>12.64</v>
       </c>
       <c r="B14">
         <f t="shared" si="3"/>
-        <v>238.28435266084193</v>
+        <v>237.34177215189871</v>
       </c>
       <c r="F14">
-        <v>14742</v>
+        <v>10245</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>12.57</v>
+        <v>12.78</v>
       </c>
       <c r="B15">
         <f t="shared" si="3"/>
-        <v>238.6634844868735</v>
+        <v>234.74178403755869</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>12.36</v>
+        <v>12.78</v>
       </c>
       <c r="B16">
         <f t="shared" si="3"/>
-        <v>242.71844660194179</v>
+        <v>234.74178403755869</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1416,7 +1660,7 @@
       </c>
       <c r="B17" s="3">
         <f>AVERAGE(B12:B16)</f>
-        <v>240.20295091119186</v>
+        <v>235.07847553954838</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1425,14 +1669,14 @@
       </c>
       <c r="B18" s="5">
         <f>STDEV(B12:B16)</f>
-        <v>1.8021287650322444</v>
+        <v>1.287428073243424</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F18" s="3">
         <f>AVERAGE(F12:F16)</f>
-        <v>14497.333333333334</v>
+        <v>10461.666666666666</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1441,7 +1685,7 @@
       </c>
       <c r="F19" s="5">
         <f>STDEV(F12:F16)</f>
-        <v>547.65074028374454</v>
+        <v>215.50947388301361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Various sims for John
</commit_message>
<xml_diff>
--- a/Experimental Results/dilution rate measurements.xlsx
+++ b/Experimental Results/dilution rate measurements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="135" windowWidth="14340" windowHeight="5835"/>
+    <workbookView xWindow="396" yWindow="132" windowWidth="14340" windowHeight="5832" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="10_22" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="11_2" sheetId="3" r:id="rId3"/>
     <sheet name="11_5" sheetId="4" r:id="rId4"/>
     <sheet name="11_12" sheetId="5" r:id="rId5"/>
+    <sheet name="Methane Standard Curve" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="33">
   <si>
     <t>Liters</t>
   </si>
@@ -75,13 +76,55 @@
   </si>
   <si>
     <t xml:space="preserve">OD: </t>
+  </si>
+  <si>
+    <t>Methane %</t>
+  </si>
+  <si>
+    <t>Area 1</t>
+  </si>
+  <si>
+    <t>Area 2</t>
+  </si>
+  <si>
+    <t>Area 3</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Stdev</t>
+  </si>
+  <si>
+    <t>Slope</t>
+  </si>
+  <si>
+    <t>Y-intercept</t>
+  </si>
+  <si>
+    <t>w/o 100%</t>
+  </si>
+  <si>
+    <t>W/ 100%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% Methane: </t>
+  </si>
+  <si>
+    <t>Methane Amount (mL/min):</t>
+  </si>
+  <si>
+    <t>Methane Amount (mmol/min):</t>
+  </si>
+  <si>
+    <t>Methane Amount (mmol/h)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +140,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -106,7 +156,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -158,11 +208,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -170,9 +239,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -182,6 +255,216 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Methane Standard Curve'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.5242782152230968E-3"/>
+                  <c:y val="-0.16702573636628754"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Methane Standard Curve'!$E$2:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5.0433333333333339</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>605.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1502.5333333333335</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2821.9333333333329</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4092.2000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5239.7333333333327</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23749</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Methane Standard Curve'!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.996007984031936E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.9840637450199202E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0347887823926161E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.0068022390703611E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0076012020505568E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.0010971303185108E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="159896320"/>
+        <c:axId val="150531072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="159896320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="150531072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="150531072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="159896320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -471,22 +754,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -494,12 +777,12 @@
         <v>0.626</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -516,7 +799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f>26+20/60</f>
         <v>26.333333333333332</v>
@@ -543,7 +826,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>22+1/12</f>
         <v>22.083333333333332</v>
@@ -564,7 +847,7 @@
         <v>8.0313278746885014E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <f>25+10/60</f>
         <v>25.166666666666668</v>
@@ -585,7 +868,7 @@
         <v>8.2469074097213532E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
@@ -594,7 +877,7 @@
         <v>8.1391176422049266E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="4" t="s">
         <v>17</v>
       </c>
@@ -603,7 +886,7 @@
         <v>1.5243775110677241E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -611,7 +894,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -622,7 +905,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12.84</v>
       </c>
@@ -634,7 +917,7 @@
         <v>14540</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12.7</v>
       </c>
@@ -646,7 +929,7 @@
         <v>14297</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12.55</v>
       </c>
@@ -658,7 +941,7 @@
         <v>14693</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12.36</v>
       </c>
@@ -667,7 +950,7 @@
         <v>242.71844660194179</v>
       </c>
     </row>
-    <row r="16" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>12.93</v>
       </c>
@@ -676,7 +959,7 @@
         <v>232.01856148491879</v>
       </c>
     </row>
-    <row r="17" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -685,7 +968,7 @@
         <v>236.72923300841694</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>14</v>
       </c>
@@ -701,13 +984,49 @@
         <v>14510</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E19" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F19" s="5">
         <f>STDEV(F12:F14)</f>
         <v>199.69727088771143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="7">
+        <f>F18*'Methane Standard Curve'!B13+'Methane Standard Curve'!C13</f>
+        <v>2.4971655045194385E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <f>B17*F21</f>
+        <v>5.9115207457996322</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24">
+        <f>B23/22.4</f>
+        <v>0.26390717615176928</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <f>B24*60</f>
+        <v>15.834430569106157</v>
       </c>
     </row>
   </sheetData>
@@ -717,22 +1036,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="A1:F20"/>
+      <selection activeCell="A21" sqref="A21:F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -740,12 +1059,12 @@
         <v>0.67200000000000004</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -762,7 +1081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <f>25+55/60</f>
         <v>25.916666666666668</v>
@@ -786,7 +1105,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>23+23/60</f>
         <v>23.383333333333333</v>
@@ -807,7 +1126,7 @@
         <v>9.9248241638537363E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>24</v>
       </c>
@@ -827,7 +1146,7 @@
         <v>8.4119496855345893E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
@@ -836,7 +1155,7 @@
         <v>9.0243491953218014E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="4" t="s">
         <v>17</v>
       </c>
@@ -845,7 +1164,7 @@
         <v>7.96516101052323E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -853,7 +1172,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -864,7 +1183,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12.25</v>
       </c>
@@ -876,7 +1195,7 @@
         <v>14371</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11.74</v>
       </c>
@@ -888,7 +1207,7 @@
         <v>14899</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12.08</v>
       </c>
@@ -900,7 +1219,7 @@
         <v>11940</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12.4</v>
       </c>
@@ -912,7 +1231,7 @@
         <v>13665</v>
       </c>
     </row>
-    <row r="16" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>11.83</v>
       </c>
@@ -924,7 +1243,7 @@
         <v>14210</v>
       </c>
     </row>
-    <row r="17" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -933,7 +1252,7 @@
         <v>248.86140042339238</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>14</v>
       </c>
@@ -949,13 +1268,49 @@
         <v>13817</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E19" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F19" s="5">
         <f>STDEV(F12:F16)</f>
         <v>1137.7963350266164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="7">
+        <f>F18*'Methane Standard Curve'!B13+'Methane Standard Curve'!C13</f>
+        <v>2.3830077808006077E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <f>B17*F21</f>
+        <v>5.9303865354987968</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24">
+        <f>B23/22.4</f>
+        <v>0.26474939890619631</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <f>B24*60</f>
+        <v>15.884963934371779</v>
       </c>
     </row>
   </sheetData>
@@ -965,22 +1320,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -988,12 +1343,12 @@
         <v>0.71199999999999997</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1010,7 +1365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <f>22+50/60</f>
         <v>22.833333333333332</v>
@@ -1034,7 +1389,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>20+0.25</f>
         <v>20.25</v>
@@ -1055,7 +1410,7 @@
         <v>9.0379687863964595E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>49+50/60</f>
         <v>49.833333333333336</v>
@@ -1076,7 +1431,7 @@
         <v>8.8597210828547976E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>24</v>
       </c>
@@ -1096,7 +1451,7 @@
         <v>9.2767295597484298E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1105,7 +1460,7 @@
         <v>8.9214109445657191E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D9" s="4" t="s">
         <v>17</v>
       </c>
@@ -1114,7 +1469,7 @@
         <v>3.2243641791387537E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1122,7 +1477,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1133,7 +1488,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12.73</v>
       </c>
@@ -1145,7 +1500,7 @@
         <v>14866</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12.7</v>
       </c>
@@ -1157,7 +1512,7 @@
         <v>15913</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12.77</v>
       </c>
@@ -1169,7 +1524,7 @@
         <v>11486</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>12.65</v>
       </c>
@@ -1178,7 +1533,7 @@
         <v>237.15415019762844</v>
       </c>
     </row>
-    <row r="17" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>12.67</v>
       </c>
@@ -1187,7 +1542,7 @@
         <v>236.77979479084453</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -1196,7 +1551,7 @@
         <v>236.1487621304139</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>14</v>
       </c>
@@ -1212,13 +1567,49 @@
         <v>14088.333333333334</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E20" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F20" s="5">
         <f>STDEV(F13:F17)</f>
         <v>2313.6889015883949</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="7">
+        <f>F19*'Methane Standard Curve'!B13+'Methane Standard Curve'!C13</f>
+        <v>2.4277044556958109E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24">
+        <f>B18*F22</f>
+        <v>5.73299402031056</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25">
+        <f>B24/22.4</f>
+        <v>0.25593723304957861</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26">
+        <f>B25*60</f>
+        <v>15.356233982974716</v>
       </c>
     </row>
   </sheetData>
@@ -1228,22 +1619,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -1251,12 +1642,12 @@
         <v>0.67200000000000004</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1273,7 +1664,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <f>24+7+3/4</f>
         <v>31.75</v>
@@ -1297,7 +1688,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>24+40/60</f>
         <v>24.666666666666668</v>
@@ -1318,7 +1709,7 @@
         <v>4.7807241203467625E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <f>48+20+0.25</f>
         <v>68.25</v>
@@ -1339,7 +1730,7 @@
         <v>4.616766880917824E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1348,7 +1739,7 @@
         <v>4.538924970510174E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="4" t="s">
         <v>17</v>
       </c>
@@ -1357,7 +1748,7 @@
         <v>2.8870105582736597E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1365,7 +1756,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1376,7 +1767,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12.48</v>
       </c>
@@ -1388,7 +1779,7 @@
         <v>13870</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12.45</v>
       </c>
@@ -1400,7 +1791,7 @@
         <v>14880</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12.59</v>
       </c>
@@ -1412,7 +1803,7 @@
         <v>14742</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12.57</v>
       </c>
@@ -1421,7 +1812,7 @@
         <v>238.6634844868735</v>
       </c>
     </row>
-    <row r="16" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>12.36</v>
       </c>
@@ -1430,7 +1821,7 @@
         <v>242.71844660194179</v>
       </c>
     </row>
-    <row r="17" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -1439,7 +1830,7 @@
         <v>240.20295091119186</v>
       </c>
     </row>
-    <row r="18" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>14</v>
       </c>
@@ -1455,13 +1846,49 @@
         <v>14497.333333333334</v>
       </c>
     </row>
-    <row r="19" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E19" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F19" s="5">
         <f>STDEV(F12:F16)</f>
         <v>547.65074028374454</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="7">
+        <f>F18*'Methane Standard Curve'!B13+'Methane Standard Curve'!C13</f>
+        <v>2.4950789275587283E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <f>B17*F21</f>
+        <v>5.9932532115593844</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24">
+        <f>B23/22.4</f>
+        <v>0.26755594694461537</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <f>B24*60</f>
+        <v>16.053356816676924</v>
       </c>
     </row>
   </sheetData>
@@ -1471,22 +1898,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -1494,12 +1921,12 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1516,26 +1943,30 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>48.25</v>
+      </c>
+      <c r="B4" s="6">
+        <v>5.95</v>
+      </c>
       <c r="C4" s="6">
         <f>B4/2.65</f>
-        <v>0</v>
-      </c>
-      <c r="D4" s="6" t="e">
+        <v>2.2452830188679247</v>
+      </c>
+      <c r="D4" s="6">
         <f>A4/C4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E4" s="6" t="e">
+        <v>21.489495798319325</v>
+      </c>
+      <c r="E4" s="6">
         <f>1/D4</f>
-        <v>#DIV/0!</v>
+        <v>4.6534363085345594E-2</v>
       </c>
       <c r="F4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C5">
         <f t="shared" ref="C5:C6" si="0">B5/2.65</f>
         <v>0</v>
@@ -1549,7 +1980,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1563,7 +1994,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1572,7 +2003,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="4" t="s">
         <v>17</v>
       </c>
@@ -1581,7 +2012,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1589,7 +2020,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1600,7 +2031,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12.8</v>
       </c>
@@ -1612,7 +2043,7 @@
         <v>10464</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12.81</v>
       </c>
@@ -1624,7 +2055,7 @@
         <v>10676</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12.64</v>
       </c>
@@ -1636,7 +2067,7 @@
         <v>10245</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12.78</v>
       </c>
@@ -1645,7 +2076,7 @@
         <v>234.74178403755869</v>
       </c>
     </row>
-    <row r="16" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>12.78</v>
       </c>
@@ -1654,7 +2085,7 @@
         <v>234.74178403755869</v>
       </c>
     </row>
-    <row r="17" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -1663,7 +2094,7 @@
         <v>235.07847553954838</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>14</v>
       </c>
@@ -1679,7 +2110,7 @@
         <v>10461.666666666666</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E19" s="4" t="s">
         <v>15</v>
       </c>
@@ -1688,7 +2119,303 @@
         <v>215.50947388301361</v>
       </c>
     </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="7">
+        <f>F18*'Methane Standard Curve'!B13+'Methane Standard Curve'!C13</f>
+        <v>1.8302845258925997E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <f>B17*F21</f>
+        <v>4.3026049615045743</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24">
+        <f>B23/22.4</f>
+        <v>0.19208057863859707</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <f>B24*60</f>
+        <v>11.524834718315823</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <f>0/28</f>
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>15.13</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>AVERAGE(B2:D2)</f>
+        <v>5.0433333333333339</v>
+      </c>
+      <c r="F2">
+        <f>STDEV(B2:D2)</f>
+        <v>8.7353095728390375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <f>0.056/28.056</f>
+        <v>1.996007984031936E-3</v>
+      </c>
+      <c r="B3">
+        <v>619.20000000000005</v>
+      </c>
+      <c r="C3">
+        <v>598.70000000000005</v>
+      </c>
+      <c r="D3">
+        <v>597.70000000000005</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E9" si="0">AVERAGE(B3:D3)</f>
+        <v>605.20000000000005</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F9" si="1">STDEV(B3:D3)</f>
+        <v>12.134661099511597</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <f>0.112/28.112</f>
+        <v>3.9840637450199202E-3</v>
+      </c>
+      <c r="B4">
+        <v>1474.2</v>
+      </c>
+      <c r="C4">
+        <v>1505.6</v>
+      </c>
+      <c r="D4">
+        <v>1527.8</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>1502.5333333333335</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>26.931270548069776</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <f>0.17/28.17</f>
+        <v>6.0347887823926161E-3</v>
+      </c>
+      <c r="B5">
+        <v>2848.5</v>
+      </c>
+      <c r="C5">
+        <v>2757.7</v>
+      </c>
+      <c r="D5">
+        <v>2859.6</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>2821.9333333333329</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>55.90387583462654</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <f>0.226/28.226</f>
+        <v>8.0068022390703611E-3</v>
+      </c>
+      <c r="B6">
+        <v>4096.3</v>
+      </c>
+      <c r="C6">
+        <v>3929.5</v>
+      </c>
+      <c r="D6">
+        <v>4250.8</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>4092.2000000000003</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>160.68923423801618</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <f>0.285/28.285</f>
+        <v>1.0076012020505568E-2</v>
+      </c>
+      <c r="B7">
+        <v>5090.3</v>
+      </c>
+      <c r="C7">
+        <v>5249</v>
+      </c>
+      <c r="D7">
+        <v>5379.9</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>5239.7333333333327</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>145.02221668879997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <f>1.167/29.167</f>
+        <v>4.0010971303185108E-2</v>
+      </c>
+      <c r="B8">
+        <v>23393</v>
+      </c>
+      <c r="C8">
+        <v>23387</v>
+      </c>
+      <c r="D8">
+        <v>24467</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>23749</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>621.81347685620324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <f>28/28</f>
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>167429</v>
+      </c>
+      <c r="C9">
+        <v>167356</v>
+      </c>
+      <c r="D9">
+        <v>164347</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>166377.33333333334</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>1758.6990456963729</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="9">
+        <f>SLOPE(A2:A8,E2:E8)</f>
+        <v>1.6472976005603261E-6</v>
+      </c>
+      <c r="C13" s="5">
+        <f>INTERCEPT(A2:A8,E2:E8)</f>
+        <v>1.0693668610640503E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14">
+        <f>SLOPE(A2:A9,E2:E9)</f>
+        <v>6.0705449754459408E-6</v>
+      </c>
+      <c r="C14">
+        <f>INTERCEPT(A2:A9,E2:E9)</f>
+        <v>-2.1333513930758413E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added summary to ATPM data
</commit_message>
<xml_diff>
--- a/Experimental Results/dilution rate measurements.xlsx
+++ b/Experimental Results/dilution rate measurements.xlsx
@@ -4,24 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="135" windowWidth="14340" windowHeight="5835" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="390" yWindow="135" windowWidth="14340" windowHeight="5835" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
-    <sheet name="10_22" sheetId="1" r:id="rId1"/>
-    <sheet name="10_27" sheetId="2" r:id="rId2"/>
-    <sheet name="11_2" sheetId="3" r:id="rId3"/>
-    <sheet name="11_5" sheetId="4" r:id="rId4"/>
-    <sheet name="11_12" sheetId="5" r:id="rId5"/>
-    <sheet name="11_19" sheetId="7" r:id="rId6"/>
-    <sheet name="Methane Standard Curve" sheetId="6" r:id="rId7"/>
-    <sheet name="Compilation" sheetId="8" r:id="rId8"/>
+    <sheet name="Summary of Results" sheetId="10" r:id="rId1"/>
+    <sheet name="10_22" sheetId="1" r:id="rId2"/>
+    <sheet name="10_27" sheetId="2" r:id="rId3"/>
+    <sheet name="11_2" sheetId="3" r:id="rId4"/>
+    <sheet name="11_5" sheetId="4" r:id="rId5"/>
+    <sheet name="11_12" sheetId="5" r:id="rId6"/>
+    <sheet name="11_19" sheetId="7" r:id="rId7"/>
+    <sheet name="Methane Standard Curve" sheetId="6" r:id="rId8"/>
+    <sheet name="Compilation" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="65">
   <si>
     <t>Liters</t>
   </si>
@@ -189,6 +190,33 @@
   </si>
   <si>
     <t>His yield w/my #s</t>
+  </si>
+  <si>
+    <t>Growth Rate (1/h)</t>
+  </si>
+  <si>
+    <t>MER (mmol/gDCW/h)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yield </t>
+  </si>
+  <si>
+    <t>Yield Types</t>
+  </si>
+  <si>
+    <t>Dil. Rate + New OD</t>
+  </si>
+  <si>
+    <t>DT + New OD</t>
+  </si>
+  <si>
+    <t>Dil. Rate + Old OD</t>
+  </si>
+  <si>
+    <t>DT + Old OD</t>
+  </si>
+  <si>
+    <t>Growth, Methane Production, and Yield</t>
   </si>
 </sst>
 </file>
@@ -233,7 +261,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -318,12 +346,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -340,6 +420,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,6 +449,204 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Fitted Growth Data</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.19854203708407417"/>
+                  <c:y val="3.595533609146314E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Compilation!$B$8:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>9.0243491953218014E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.9214109445657191E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.6534363085345594E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0487379671178976E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Compilation!$C$8:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>35.815665436444306</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.678400542591753</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.038398536538562</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.475688694632385</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="58037376"/>
+        <c:axId val="58038912"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="58037376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Growth Rate (1/h)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="58038912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="58038912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>MER (mmol/gDCW/h)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="58037376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -482,11 +773,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="54219904"/>
-        <c:axId val="54221440"/>
+        <c:axId val="42181760"/>
+        <c:axId val="42183296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54219904"/>
+        <c:axId val="42181760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -496,12 +787,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54221440"/>
+        <c:crossAx val="42183296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="54221440"/>
+        <c:axId val="42183296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -513,7 +804,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54219904"/>
+        <c:crossAx val="42181760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -530,7 +821,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -619,11 +910,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="54283264"/>
-        <c:axId val="54293248"/>
+        <c:axId val="42200448"/>
+        <c:axId val="41174144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54283264"/>
+        <c:axId val="42200448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -633,12 +924,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54293248"/>
+        <c:crossAx val="41174144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="54293248"/>
+        <c:axId val="41174144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -649,7 +940,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54283264"/>
+        <c:crossAx val="42200448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -667,6 +958,43 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -701,7 +1029,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1023,6 +1351,236 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="20"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
+        <v>42304</v>
+      </c>
+      <c r="B3" s="16">
+        <v>9.0243491953218014E-2</v>
+      </c>
+      <c r="C3" s="16">
+        <v>35.815665436444306</v>
+      </c>
+      <c r="D3" s="16">
+        <f>B3/C3*1000</f>
+        <v>2.5196653713821706</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>42310</v>
+      </c>
+      <c r="B4" s="16">
+        <v>8.9214109445657191E-2</v>
+      </c>
+      <c r="C4" s="16">
+        <v>32.678400542591753</v>
+      </c>
+      <c r="D4" s="16">
+        <f>B4/C4*1000</f>
+        <v>2.730063527111096</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
+        <v>42313</v>
+      </c>
+      <c r="B5" s="22">
+        <v>4.538924970510174E-2</v>
+      </c>
+      <c r="C5" s="22">
+        <v>36.195339142940391</v>
+      </c>
+      <c r="D5" s="16">
+        <f>B5/C5*1000</f>
+        <v>1.2540081341924529</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
+        <v>42320</v>
+      </c>
+      <c r="B6" s="16">
+        <v>4.6534363085345594E-2</v>
+      </c>
+      <c r="C6" s="16">
+        <v>21.038398536538562</v>
+      </c>
+      <c r="D6" s="16">
+        <f>B6/C6*1000</f>
+        <v>2.2118776295889044</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
+        <v>42327</v>
+      </c>
+      <c r="B7" s="16">
+        <v>7.0487379671178976E-2</v>
+      </c>
+      <c r="C7" s="16">
+        <v>30.475688694632385</v>
+      </c>
+      <c r="D7" s="16">
+        <f>B7/C7*1000</f>
+        <v>2.3129052267683048</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
+        <v>42304</v>
+      </c>
+      <c r="B11" s="16">
+        <v>2.5196653713821706</v>
+      </c>
+      <c r="C11" s="16">
+        <f>B11/LN(2)</f>
+        <v>3.6351087359927061</v>
+      </c>
+      <c r="D11" s="16">
+        <f>B11/0.66*0.34</f>
+        <v>1.2980094337423302</v>
+      </c>
+      <c r="E11" s="16">
+        <f>D11/LN(2)</f>
+        <v>1.8726317730871513</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="17">
+        <v>42310</v>
+      </c>
+      <c r="B12" s="16">
+        <v>2.730063527111096</v>
+      </c>
+      <c r="C12" s="16">
+        <f t="shared" ref="C12:C14" si="0">B12/LN(2)</f>
+        <v>3.9386491118750104</v>
+      </c>
+      <c r="D12" s="16">
+        <f t="shared" ref="D12:D14" si="1">B12/0.66*0.34</f>
+        <v>1.4063963624511708</v>
+      </c>
+      <c r="E12" s="16">
+        <f t="shared" ref="E12:E14" si="2">D12/LN(2)</f>
+        <v>2.0290010576325814</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
+        <v>42320</v>
+      </c>
+      <c r="B13" s="16">
+        <v>2.2118776295889044</v>
+      </c>
+      <c r="C13" s="16">
+        <f t="shared" si="0"/>
+        <v>3.191064887261148</v>
+      </c>
+      <c r="D13" s="16">
+        <f t="shared" si="1"/>
+        <v>1.1394521122124659</v>
+      </c>
+      <c r="E13" s="16">
+        <f t="shared" si="2"/>
+        <v>1.6438819116193792</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
+        <v>42327</v>
+      </c>
+      <c r="B14" s="16">
+        <v>2.3129052267683048</v>
+      </c>
+      <c r="C14" s="16">
+        <f t="shared" si="0"/>
+        <v>3.3368169007047968</v>
+      </c>
+      <c r="D14" s="16">
+        <f t="shared" si="1"/>
+        <v>1.191496631971551</v>
+      </c>
+      <c r="E14" s="16">
+        <f t="shared" si="2"/>
+        <v>1.718966282181259</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1312,7 +1870,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
@@ -1661,7 +2219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
@@ -2025,12 +2583,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2369,7 +2927,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
@@ -2673,12 +3231,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30:G31"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3050,7 +3608,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
@@ -3310,12 +3868,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>